<commit_message>
v4 : multi-obj avec intlinprog
</commit_message>
<xml_diff>
--- a/Donnees_Projet_Optimisation.xlsx
+++ b/Donnees_Projet_Optimisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20380"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dirion/Desktop/Enseignement 2020/ETN/Projet optimisation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emac\Desktop\Optimisation\Projet Optim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A0ACFD-B154-8C4C-A30A-7FEEA9C0DA85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BA0E5B-60CB-47C4-AE62-E421A9C27759}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="16800" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="465" windowWidth="25035" windowHeight="16800" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau1" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Unit</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>RampDownRate_MWmin_1</t>
+  </si>
+  <si>
+    <t>Emissions</t>
   </si>
 </sst>
 </file>
@@ -404,7 +407,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -467,6 +470,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -936,9 +945,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="32" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="28.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -946,7 +955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -954,7 +963,7 @@
         <v>1775.835</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -962,7 +971,7 @@
         <v>1669.8150000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -970,7 +979,7 @@
         <v>1590.3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -978,7 +987,7 @@
         <v>1563.7950000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -986,7 +995,7 @@
         <v>1563.7950000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -994,7 +1003,7 @@
         <v>1590.3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>1961.37</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>2279.4299999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>9</v>
       </c>
@@ -1018,7 +1027,7 @@
         <v>2517.9749999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>10</v>
       </c>
@@ -1026,7 +1035,7 @@
         <v>2544.48</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>11</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>2544.48</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>12</v>
       </c>
@@ -1042,7 +1051,7 @@
         <v>2517.9749999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1050,7 +1059,7 @@
         <v>2517.9749999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>14</v>
       </c>
@@ -1058,7 +1067,7 @@
         <v>2517.9749999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>15</v>
       </c>
@@ -1066,7 +1075,7 @@
         <v>2517.9749999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>16</v>
       </c>
@@ -1074,7 +1083,7 @@
         <v>2517.9749999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>17</v>
       </c>
@@ -1082,7 +1091,7 @@
         <v>2623.9949999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="20">
         <v>18</v>
       </c>
@@ -1090,7 +1099,7 @@
         <v>2650.5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="20">
         <v>19</v>
       </c>
@@ -1098,7 +1107,7 @@
         <v>2650.5</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="20">
         <v>20</v>
       </c>
@@ -1106,7 +1115,7 @@
         <v>2544.48</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>21</v>
       </c>
@@ -1114,7 +1123,7 @@
         <v>2411.9549999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>22</v>
       </c>
@@ -1122,7 +1131,7 @@
         <v>2199.915</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>23</v>
       </c>
@@ -1130,7 +1139,7 @@
         <v>1934.865</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
         <v>24</v>
       </c>
@@ -1150,21 +1159,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="7" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="8.625" customWidth="1"/>
+    <col min="5" max="7" width="9.625" customWidth="1"/>
+    <col min="19" max="19" width="11.625" customWidth="1"/>
+    <col min="21" max="21" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:18" ht="62" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:21" ht="42" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,8 +1230,14 @@
       <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -1275,8 +1292,14 @@
       <c r="R3" s="17">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" s="20">
+        <v>888</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1331,8 +1354,14 @@
       <c r="R4" s="17">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" s="20">
+        <v>888</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1387,8 +1416,14 @@
       <c r="R5" s="17">
         <v>-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5" s="20">
+        <v>733</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1443,8 +1478,14 @@
       <c r="R6" s="17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S6" s="23">
+        <v>733</v>
+      </c>
+      <c r="U6" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1499,8 +1540,14 @@
       <c r="R7" s="17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S7" s="23">
+        <v>733</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1555,8 +1602,14 @@
       <c r="R8" s="17">
         <v>-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S8" s="23">
+        <v>888</v>
+      </c>
+      <c r="U8" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1611,8 +1664,14 @@
       <c r="R9" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S9" s="23">
+        <v>888</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1667,8 +1726,14 @@
       <c r="R10" s="17">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S10" s="23">
+        <v>29</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1723,8 +1788,14 @@
       <c r="R11" s="17">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S11" s="23">
+        <v>29</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1779,8 +1850,14 @@
       <c r="R12" s="17">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S12" s="23">
+        <v>26</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1835,8 +1912,14 @@
       <c r="R13" s="17">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="S13" s="23">
+        <v>888</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -1890,6 +1973,12 @@
       </c>
       <c r="R14" s="18">
         <v>50</v>
+      </c>
+      <c r="S14" s="23">
+        <v>888</v>
+      </c>
+      <c r="U14" s="11" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>